<commit_message>
done counting for all regions
</commit_message>
<xml_diff>
--- a/excels/Перечень_район_метеостанция.xlsx
+++ b/excels/Перечень_район_метеостанция.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Работа\2023\9_Сентябрь\ТЗ_студенты_НГУ_5.09.23\2022_районы\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Antony\NSU_Education\Meteo\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -176,9 +176,6 @@
     <t>TATARSK</t>
   </si>
   <si>
-    <t>TOGUCHIN</t>
-  </si>
-  <si>
     <t>UBINSK</t>
   </si>
   <si>
@@ -269,9 +266,6 @@
     <t>sun_tatarsk</t>
   </si>
   <si>
-    <t>sun_toguchin</t>
-  </si>
-  <si>
     <t>sun_ubinsk</t>
   </si>
   <si>
@@ -285,12 +279,18 @@
   </si>
   <si>
     <t>sun_chistoz</t>
+  </si>
+  <si>
+    <t>TOGUCHI</t>
+  </si>
+  <si>
+    <t>sun_toguchi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -840,7 +840,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -858,7 +858,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -869,7 +869,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -880,7 +880,7 @@
         <v>31</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -888,10 +888,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -902,7 +902,7 @@
         <v>34</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -910,10 +910,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -924,7 +924,7 @@
         <v>35</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -935,7 +935,7 @@
         <v>36</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -946,7 +946,7 @@
         <v>37</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -957,7 +957,7 @@
         <v>40</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -968,7 +968,7 @@
         <v>39</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -979,7 +979,7 @@
         <v>41</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -990,7 +990,7 @@
         <v>42</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -998,10 +998,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -1012,7 +1012,7 @@
         <v>43</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -1023,7 +1023,7 @@
         <v>38</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -1034,7 +1034,7 @@
         <v>44</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -1045,7 +1045,7 @@
         <v>45</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -1053,10 +1053,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -1067,7 +1067,7 @@
         <v>46</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -1078,7 +1078,7 @@
         <v>47</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -1089,7 +1089,7 @@
         <v>48</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -1100,7 +1100,7 @@
         <v>49</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -1108,10 +1108,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -1119,10 +1119,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -1130,10 +1130,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -1144,7 +1144,7 @@
         <v>32</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -1152,10 +1152,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1166,7 +1166,7 @@
         <v>33</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>